<commit_message>
consolidate (some) login/passwd ops; code secure_inetd
</commit_message>
<xml_diff>
--- a/PiHarending.xlsx
+++ b/PiHarending.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COwnby\Documents\myStuff\work\Archethought\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COwnby\Documents\VBShare\GitHub\hardening\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -432,8 +432,8 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>